<commit_message>
Predictive models and results for Capstone 1
</commit_message>
<xml_diff>
--- a/Capstone1/Datasets/codebook_publicv4.xlsx
+++ b/Capstone1/Datasets/codebook_publicv4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ishareef7/Springboard/Capstone1/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AA5596-AA89-EB4E-856E-8DB56C2F28F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2199A57C-C6FB-A448-90B9-FC70F5BC2D6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5204" uniqueCount="1757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5205" uniqueCount="1757">
   <si>
     <t>2015 RECS Variable and Response Codebook</t>
   </si>
@@ -8473,8 +8473,8 @@
   <dimension ref="A1:O765"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+      <pane ySplit="4" topLeftCell="A592" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F596" sqref="F596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27514,7 +27514,9 @@
         <v>1330</v>
       </c>
       <c r="E595" s="30"/>
-      <c r="F595" s="41"/>
+      <c r="F595" s="41" t="s">
+        <v>1748</v>
+      </c>
       <c r="G595" s="41" t="s">
         <v>1755</v>
       </c>

</xml_diff>